<commit_message>
Added coding MCQs to Spring Hibernate With JPA
</commit_message>
<xml_diff>
--- a/Hibernate With Jpa _AND_JSP_AND_Servlets(MCQ'S).xlsx
+++ b/Hibernate With Jpa _AND_JSP_AND_Servlets(MCQ'S).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ganesh\Desktop\mcq\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Company\TechElevate\question-bank\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5664"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16390" windowHeight="5660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="285">
   <si>
     <t>What technique is used for the authentication mechanism in the servlet specification?</t>
   </si>
@@ -780,12 +780,193 @@
   <si>
     <t>d) Local.retrieveISO3Country()</t>
   </si>
+  <si>
+    <t>EntityManager em = entityManagerFactory.createEntityManager();
+Query query = em.createQuery
+  ("SELECT e FROM Employee e WHERE e.dept IN :deptNames");
+query.setParameter("deptNames", Arrays.asList("Sales", "Admin"));
+List&lt;Employee&gt; resultList = query.getResultList();
+resultList.forEach(System.out::println);
+em.close();</t>
+  </si>
+  <si>
+    <t>Employee{id=1, name='Diana', dept='IT', salary=3000}</t>
+  </si>
+  <si>
+    <t>Employee{id=2, name='Rose', dept='Sales', salary=2000}</t>
+  </si>
+  <si>
+    <t>Employee{id=4, name='Mike', dept='HR', salary=3500}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Employee{id=3, name='Denise', dept='Admin', salary=4000}</t>
+  </si>
+  <si>
+    <t>B,D</t>
+  </si>
+  <si>
+    <t>EntityManager em = entityManagerFactory.createEntityManager();
+Query query = em.createQuery
+  ("SELECT e FROM Employee e WHERE e.name NOT LIKE 'D%'");
+List&lt;Employee&gt; resultList = query.getResultList();
+resultList.forEach(System.out::println);
+em.close();</t>
+  </si>
+  <si>
+    <t>Employee{id=4, name='Mike', dept='H_R', salary=3500}</t>
+  </si>
+  <si>
+    <t>Employee{id=3, name='Denise', dept='Admin', salary=4000}</t>
+  </si>
+  <si>
+    <t>B,C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The following code snippet is for which CRUD operation.  
+EntityManager manager = emf.createEntityManager();
+  manager.getTransaction().begin();
+  Employee emp = manager.find(Employee.class,4);
+  emp.setE_name("Luna Lovegood");
+  emp.setE_password("root");
+  emp.setE_salary(11500);
+  manager.persist(emp);
+  manager.getTransaction().commit();
+  manager.close();  </t>
+  </si>
+  <si>
+    <t>Insert</t>
+  </si>
+  <si>
+    <t>Retrive</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>EntityManager em = entityManagerFactory.createEntityManager();
+Query query = em.createQuery
+  ("SELECT e FROM Employee e WHERE e.dept IS NULL");
+List&lt;Employee&gt; resultList = query.getResultList();
+resultList.forEach(System.out::println);
+em.close();</t>
+  </si>
+  <si>
+    <t>Employee{id=4, name='Mike', dept='  ', salary=3500}</t>
+  </si>
+  <si>
+    <t>Employee{id=3, name='Denise', dept='  ', salary=4000}</t>
+  </si>
+  <si>
+    <t>A,D</t>
+  </si>
+  <si>
+    <t>The following code snippet is for which CRUD operation.
+EntityManager manager = emf.createEntityManager();
+  manager.getTransaction().begin();
+  SkillsTable st = manager.find(SkillsTable.class,2);
+  manager.remove(st);
+  manager.getTransaction().commit();
+  manager.close();</t>
+  </si>
+  <si>
+    <t>You want to write a JPA Entity class to model a 
+databank table named COOPERATE_USER.
+Each user is uniquely identified in this table by 
+his or her social security number SSN.
+Along with SSN the system keeps user name,
+job, address and birth date.
+How to declare such JPA Entity class?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write a CooperateUser public class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annotate the CooperateUser class with @Table(name=" COOPERATE_USER") </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annotate the CooperateUser class with @Entity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The CooperateUser class must implement Serializable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Define private attributes ssn, job, name, addess and birthdate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annotate the ' name' attibute with @Id </t>
+  </si>
+  <si>
+    <t>A,B,C,E</t>
+  </si>
+  <si>
+    <t>private static void findEmployeesByDept(String dept) 
+{
+ EntityManager em = entityManagerFactory.createEntityManager();
+ Query query = em.createQuery
+ ("SELECT e FROM Employee e WHERE e.dept = :deptName");
+  query.setParameter("deptName", dept);
+  List&lt;Employee&gt; resultList = query.getResultList();
+  resultList.forEach(System.out::println);
+  em.close();
+}
+public static void main(String[] args) 
+{
+ try{
+      persistEmployees();
+      findEmployeesByDept("IT");
+    }finally{
+      entityManagerFactory.close();
+    }
+}</t>
+  </si>
+  <si>
+    <t>Employee{id=1, name='Diana', dept='IT'}</t>
+  </si>
+  <si>
+    <t>Employee{id=2, name='Rose', dept='ADMIN'}</t>
+  </si>
+  <si>
+    <t>Employee{id=3, name='Denise', dept='IT'}</t>
+  </si>
+  <si>
+    <t>Employee{id=4, name='Harley', dept='ADMIN'}</t>
+  </si>
+  <si>
+    <t>A,C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> What's true about the following @Entity association between House and Window?
+@Entity
+public class Window {
+ @Id
+ private int winNo;
+ @ManyToOne
+ private House aHouse;
+}
+@Entity
+public class House {
+ @Id
+ private int houseNo;
+ @OneToMany(mappedBy="aHouse")
+ private List windows;
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> It's OneToMany unidirectional association</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> It's OneToMany bidirectional association</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -801,69 +982,51 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Bahnschrift SemiLight"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Arial"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Bahnschrift SemiLight"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <sz val="14"/>
+      <name val="Bahnschrift SemiLight"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Bahnschrift SemiLight"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <sz val="14"/>
+      <color rgb="FF045482"/>
+      <name val="Bahnschrift SemiLight"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF045482"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <sz val="14"/>
+      <color rgb="FF555555"/>
+      <name val="Bahnschrift SemiLight"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Bahnschrift SemiLight"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF555555"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
+      <sz val="14"/>
       <color rgb="FF212529"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Bahnschrift SemiLight"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -874,12 +1037,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -890,64 +1068,46 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1254,31 +1414,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:F58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="124.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="37.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.5546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="124.54296875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.36328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.54296875" style="2" customWidth="1"/>
     <col min="5" max="5" width="30" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="2"/>
+    <col min="6" max="6" width="14.90625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.08984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1287,12 +1447,12 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" ht="35" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="b">
@@ -1301,14 +1461,14 @@
       <c r="C2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:6" ht="35" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1323,11 +1483,11 @@
       <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1343,11 +1503,11 @@
       <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1363,11 +1523,11 @@
       <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1377,12 +1537,12 @@
       <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="2">
@@ -1397,11 +1557,11 @@
       <c r="E7" s="2">
         <v>7</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1417,12 +1577,12 @@
       <c r="E8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:6" ht="35" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="2" t="b">
@@ -1431,531 +1591,531 @@
       <c r="C9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:6" ht="70" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:6" ht="35" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="234" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:6" ht="262.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+    <row r="20" spans="1:6" ht="35" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="78" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
+    <row r="21" spans="1:6" ht="105" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
+    <row r="25" spans="1:6" ht="35" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
+    <row r="29" spans="1:6" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F29" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="18" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F30" s="19" t="s">
+      <c r="F30" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F31" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="16" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F33" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
+    <row r="34" spans="1:6" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F34" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="16" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="F35" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>150</v>
       </c>
@@ -1965,11 +2125,11 @@
       <c r="C36" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>154</v>
       </c>
@@ -1985,11 +2145,11 @@
       <c r="E37" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F37" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>160</v>
       </c>
@@ -2005,11 +2165,11 @@
       <c r="E38" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F38" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>164</v>
       </c>
@@ -2025,11 +2185,11 @@
       <c r="E39" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F39" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>168</v>
       </c>
@@ -2045,11 +2205,11 @@
       <c r="E40" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F40" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>172</v>
       </c>
@@ -2065,11 +2225,11 @@
       <c r="E41" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="F41" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>176</v>
       </c>
@@ -2085,11 +2245,11 @@
       <c r="E42" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F42" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="70" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>181</v>
       </c>
@@ -2105,11 +2265,11 @@
       <c r="E43" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F43" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>186</v>
       </c>
@@ -2125,11 +2285,11 @@
       <c r="E44" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F44" s="6" t="s">
+      <c r="F44" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="70" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>192</v>
       </c>
@@ -2145,11 +2305,11 @@
       <c r="E45" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="F45" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>197</v>
       </c>
@@ -2165,11 +2325,11 @@
       <c r="E46" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="F46" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>202</v>
       </c>
@@ -2179,11 +2339,11 @@
       <c r="C47" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="F47" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>203</v>
       </c>
@@ -2193,11 +2353,11 @@
       <c r="C48" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="F48" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>204</v>
       </c>
@@ -2213,11 +2373,11 @@
       <c r="E49" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="F49" s="6" t="s">
+      <c r="F49" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>209</v>
       </c>
@@ -2233,11 +2393,11 @@
       <c r="E50" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="F50" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>214</v>
       </c>
@@ -2253,11 +2413,11 @@
       <c r="E51" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="F51" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>219</v>
       </c>
@@ -2273,11 +2433,11 @@
       <c r="E52" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="F52" s="6" t="s">
+      <c r="F52" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>224</v>
       </c>
@@ -2287,11 +2447,11 @@
       <c r="C53" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="F53" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>227</v>
       </c>
@@ -2307,11 +2467,11 @@
       <c r="E54" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="F54" s="6" t="s">
+      <c r="F54" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>232</v>
       </c>
@@ -2327,11 +2487,11 @@
       <c r="E55" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="F55" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>237</v>
       </c>
@@ -2347,11 +2507,11 @@
       <c r="E56" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="F56" s="6" t="s">
+      <c r="F56" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>242</v>
       </c>
@@ -2361,11 +2521,11 @@
       <c r="C57" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="F57" s="6" t="s">
+      <c r="F57" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="52.5" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>243</v>
       </c>
@@ -2381,8 +2541,180 @@
       <c r="E58" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="F58" s="6" t="s">
+      <c r="F58" s="2" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="122.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="105" x14ac:dyDescent="0.35">
+      <c r="A60" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="175" x14ac:dyDescent="0.35">
+      <c r="A61" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="105" x14ac:dyDescent="0.35">
+      <c r="A62" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="122.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="122.5" x14ac:dyDescent="0.35">
+      <c r="A64" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="H64" s="13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="332.5" x14ac:dyDescent="0.35">
+      <c r="A65" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="262.5" x14ac:dyDescent="0.35">
+      <c r="A66" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="13" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2400,7 +2732,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2412,7 +2744,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>